<commit_message>
Deployed c892aabc with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/Manual/source/tab/connectors.xlsx
+++ b/Manual/source/tab/connectors.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="27"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="59"/>
   </bookViews>
   <sheets>
     <sheet name="rozcestnik" sheetId="1" state="visible" r:id="rId3"/>
@@ -65,13 +65,13 @@
     <sheet name="X10_CAN_8pin_ClikMate" sheetId="55" state="visible" r:id="rId57"/>
     <sheet name="X11_FB3_10pin_ClikMate" sheetId="56" state="visible" r:id="rId58"/>
     <sheet name="X12_UDP_8pin_ClikMate" sheetId="57" state="visible" r:id="rId59"/>
-    <sheet name="X2_ACIN_7pin_2636" sheetId="58" state="visible" r:id="rId60"/>
-    <sheet name="X6_TGS560_50_DCbus" sheetId="59" state="visible" r:id="rId61"/>
-    <sheet name="X4_TGS560_24V_5pin_BCZ" sheetId="60" state="visible" r:id="rId62"/>
+    <sheet name="X1_ACIN_7pin_2636" sheetId="58" state="visible" r:id="rId60"/>
+    <sheet name="X4_TGS560_50_DCbus" sheetId="59" state="visible" r:id="rId61"/>
+    <sheet name="X3_TGS560_24V_5pin_BCZ" sheetId="60" state="visible" r:id="rId62"/>
     <sheet name="S1_TGS560_DIP" sheetId="61" state="visible" r:id="rId63"/>
     <sheet name="LED_TGS560" sheetId="62" state="visible" r:id="rId64"/>
-    <sheet name="X4_ACIN_4pin_TGS560_25" sheetId="63" state="visible" r:id="rId65"/>
-    <sheet name="X1_DC_6pin_TGS560_25" sheetId="64" state="visible" r:id="rId66"/>
+    <sheet name="X1_ACIN_4pin_TGS560_25" sheetId="63" state="visible" r:id="rId65"/>
+    <sheet name="X4_DC_6pin_TGS560_25" sheetId="64" state="visible" r:id="rId66"/>
     <sheet name="X5_RBR_3pin_TGS560_25" sheetId="65" state="visible" r:id="rId67"/>
     <sheet name="X0a_48-100-xyz" sheetId="66" state="visible" r:id="rId68"/>
     <sheet name="X0b_48-100-xyz" sheetId="67" state="visible" r:id="rId69"/>
@@ -2095,8 +2095,8 @@
   </sheetPr>
   <dimension ref="A1:L204"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A166" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H190" activeCellId="0" sqref="H190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.2734375" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13304,7 +13304,7 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
     </sheetView>
   </sheetViews>
@@ -17780,7 +17780,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18386,8 +18386,8 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K14" activeCellId="0" sqref="K14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G34" activeCellId="0" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Deployed 4427985f with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/Manual/source/tab/connectors.xlsx
+++ b/Manual/source/tab/connectors.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="59"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="40"/>
   </bookViews>
   <sheets>
     <sheet name="rozcestnik" sheetId="1" state="visible" r:id="rId3"/>
@@ -48,7 +48,7 @@
     <sheet name="X15_BR2_4pin_LSF" sheetId="38" state="visible" r:id="rId40"/>
     <sheet name="X1_ACIN_PC5" sheetId="39" state="visible" r:id="rId41"/>
     <sheet name="X2_DC_8pin_PC5" sheetId="40" state="visible" r:id="rId42"/>
-    <sheet name="X3_DO_4pin_BCZ" sheetId="41" state="visible" r:id="rId43"/>
+    <sheet name="X2_DO_4pin_BCZ" sheetId="41" state="visible" r:id="rId43"/>
     <sheet name="X3_24V_BLF_2_5" sheetId="42" state="visible" r:id="rId44"/>
     <sheet name="X5_DI_10pin_B2CF" sheetId="43" state="visible" r:id="rId45"/>
     <sheet name="X10_DO_10pin_B2CF" sheetId="44" state="visible" r:id="rId46"/>
@@ -15056,8 +15056,8 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17936,7 +17936,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="H40" activeCellId="0" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18386,8 +18386,8 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G34" activeCellId="0" sqref="G34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Deployed 54c7106c with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/Manual/source/tab/connectors.xlsx
+++ b/Manual/source/tab/connectors.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="53"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="51"/>
   </bookViews>
   <sheets>
     <sheet name="rozcestnik" sheetId="1" state="visible" r:id="rId3"/>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2314" uniqueCount="570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2336" uniqueCount="574">
   <si>
     <t xml:space="preserve">Toto je sešit se zdrojovými tabulkami popisu konektorů TGZ/TGS v češtině. Každý list odpovídá jednomu unikátnímu typu konektoru. Jelikož se často konektory v rámci TGZ opakují (typicky ty na řídicií desce), jsou zde jen jednou. Tj. Např. IO konektor 22pin weidmuller B2CF se používá pořád dokola, je zde tedy zanesen jen jednou jako „X8_IO_22pin_B2CF“</t>
   </si>
@@ -1350,6 +1350,18 @@
     <t xml:space="preserve">RxD-</t>
   </si>
   <si>
+    <t xml:space="preserve">Hengstler Acuro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UB+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UB-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hengstler ACURO link</t>
+  </si>
+  <si>
     <t xml:space="preserve">AIN</t>
   </si>
   <si>
@@ -1797,37 +1809,37 @@
     <t xml:space="preserve">Externí P1000</t>
   </si>
   <si>
-    <t xml:space="preserve">EXC+</t>
+    <t xml:space="preserve">R2</t>
   </si>
   <si>
     <t xml:space="preserve">Buzení resolveru +</t>
   </si>
   <si>
-    <t xml:space="preserve">EXC-</t>
+    <t xml:space="preserve">R1</t>
   </si>
   <si>
     <t xml:space="preserve">Buzení resolveru -</t>
   </si>
   <si>
-    <t xml:space="preserve">SIN+</t>
+    <t xml:space="preserve">S1</t>
   </si>
   <si>
     <t xml:space="preserve">Výstup resolver SIN +</t>
   </si>
   <si>
-    <t xml:space="preserve">SIN-</t>
+    <t xml:space="preserve">S3</t>
   </si>
   <si>
     <t xml:space="preserve">Výstup resolver SIN -</t>
   </si>
   <si>
-    <t xml:space="preserve">COS+</t>
+    <t xml:space="preserve">S2</t>
   </si>
   <si>
     <t xml:space="preserve">Výstup resolver COS +</t>
   </si>
   <si>
-    <t xml:space="preserve">COS-</t>
+    <t xml:space="preserve">S4</t>
   </si>
   <si>
     <t xml:space="preserve">Výstup resolver COS -</t>
@@ -2200,7 +2212,7 @@
   </sheetPr>
   <dimension ref="A1:L262"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A57" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G65" activeCellId="0" sqref="G65"/>
     </sheetView>
   </sheetViews>
@@ -18033,10 +18045,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18045,6 +18057,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="19.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="15.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18063,6 +18076,9 @@
       <c r="E1" s="4" t="s">
         <v>399</v>
       </c>
+      <c r="F1" s="4" t="s">
+        <v>408</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="n">
@@ -18080,6 +18096,9 @@
       <c r="E2" s="4" t="s">
         <v>235</v>
       </c>
+      <c r="F2" s="4" t="s">
+        <v>409</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="n">
@@ -18097,6 +18116,9 @@
       <c r="E3" s="4" t="s">
         <v>151</v>
       </c>
+      <c r="F3" s="4" t="s">
+        <v>410</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="n">
@@ -18114,6 +18136,9 @@
       <c r="E4" s="4" t="s">
         <v>401</v>
       </c>
+      <c r="F4" s="4" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="n">
@@ -18131,6 +18156,9 @@
       <c r="E5" s="4" t="s">
         <v>403</v>
       </c>
+      <c r="F5" s="4" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="n">
@@ -18148,6 +18176,9 @@
       <c r="E6" s="4" t="s">
         <v>401</v>
       </c>
+      <c r="F6" s="4" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="n">
@@ -18165,6 +18196,9 @@
       <c r="E7" s="4" t="s">
         <v>403</v>
       </c>
+      <c r="F7" s="4" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="n">
@@ -18182,6 +18216,9 @@
       <c r="E8" s="4" t="s">
         <v>70</v>
       </c>
+      <c r="F8" s="4" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="n">
@@ -18199,6 +18236,9 @@
       <c r="E9" s="4" t="s">
         <v>70</v>
       </c>
+      <c r="F9" s="4" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="n">
@@ -18216,6 +18256,9 @@
       <c r="E10" s="4" t="s">
         <v>218</v>
       </c>
+      <c r="F10" s="4" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="n">
@@ -18232,6 +18275,9 @@
       </c>
       <c r="E11" s="4" t="s">
         <v>151</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18253,10 +18299,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18265,6 +18311,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="19.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="15.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.98"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18283,6 +18330,9 @@
       <c r="E1" s="4" t="s">
         <v>399</v>
       </c>
+      <c r="F1" s="4" t="s">
+        <v>411</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="n">
@@ -18300,6 +18350,9 @@
       <c r="E2" s="4" t="s">
         <v>235</v>
       </c>
+      <c r="F2" s="4" t="s">
+        <v>409</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="n">
@@ -18317,6 +18370,9 @@
       <c r="E3" s="4" t="s">
         <v>151</v>
       </c>
+      <c r="F3" s="4" t="s">
+        <v>410</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="n">
@@ -18334,6 +18390,9 @@
       <c r="E4" s="4" t="s">
         <v>401</v>
       </c>
+      <c r="F4" s="4" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="n">
@@ -18351,6 +18410,9 @@
       <c r="E5" s="4" t="s">
         <v>403</v>
       </c>
+      <c r="F5" s="4" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="n">
@@ -18368,6 +18430,9 @@
       <c r="E6" s="4" t="s">
         <v>401</v>
       </c>
+      <c r="F6" s="4" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="n">
@@ -18385,6 +18450,9 @@
       <c r="E7" s="4" t="s">
         <v>403</v>
       </c>
+      <c r="F7" s="4" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="n">
@@ -18402,6 +18470,9 @@
       <c r="E8" s="4" t="s">
         <v>70</v>
       </c>
+      <c r="F8" s="4" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="n">
@@ -18419,6 +18490,9 @@
       <c r="E9" s="4" t="s">
         <v>70</v>
       </c>
+      <c r="F9" s="4" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="n">
@@ -18436,6 +18510,9 @@
       <c r="E10" s="4" t="s">
         <v>218</v>
       </c>
+      <c r="F10" s="4" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="n">
@@ -18452,6 +18529,9 @@
       </c>
       <c r="E11" s="4" t="s">
         <v>151</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18502,10 +18582,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18516,7 +18596,7 @@
         <v>160</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18524,10 +18604,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18535,10 +18615,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18546,10 +18626,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18557,10 +18637,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18568,10 +18648,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18582,7 +18662,7 @@
         <v>183</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18590,10 +18670,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18604,7 +18684,7 @@
         <v>183</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18612,10 +18692,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18626,7 +18706,7 @@
         <v>183</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18648,9 +18728,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -18671,8 +18751,8 @@
       <c r="C1" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D1" s="0" t="s">
-        <v>422</v>
+      <c r="D1" s="4" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18680,13 +18760,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>409</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>423</v>
+        <v>413</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18697,10 +18777,10 @@
         <v>160</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>410</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>424</v>
+        <v>414</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18708,13 +18788,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>412</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>425</v>
+        <v>416</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18722,13 +18802,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>412</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>424</v>
+        <v>416</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18736,13 +18816,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>415</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>425</v>
+        <v>419</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18750,13 +18830,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>415</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>424</v>
+        <v>419</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18764,13 +18844,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>427</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>428</v>
+        <v>431</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18778,13 +18858,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>430</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>424</v>
+        <v>434</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18792,13 +18872,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>432</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18806,13 +18886,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>434</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>428</v>
+        <v>438</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18820,13 +18900,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>436</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>428</v>
+        <v>440</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18834,41 +18914,17 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>438</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>428</v>
+        <v>442</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="13"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -18918,7 +18974,7 @@
         <v>199</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18929,7 +18985,7 @@
         <v>197</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18940,7 +18996,7 @@
         <v>195</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18951,7 +19007,7 @@
         <v>193</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18962,7 +19018,7 @@
         <v>191</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18973,7 +19029,7 @@
         <v>189</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18984,7 +19040,7 @@
         <v>187</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18995,7 +19051,7 @@
         <v>185</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19003,10 +19059,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19014,10 +19070,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19025,10 +19081,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19036,10 +19092,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19050,7 +19106,7 @@
         <v>177</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19061,7 +19117,7 @@
         <v>175</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19072,7 +19128,7 @@
         <v>173</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19083,7 +19139,7 @@
         <v>171</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19094,7 +19150,7 @@
         <v>169</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19105,7 +19161,7 @@
         <v>167</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
     </row>
   </sheetData>
@@ -19153,10 +19209,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19164,10 +19220,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19175,10 +19231,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19186,10 +19242,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19197,10 +19253,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19208,10 +19264,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19219,10 +19275,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19230,10 +19286,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
     </row>
   </sheetData>
@@ -19281,10 +19337,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19292,10 +19348,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19306,7 +19362,7 @@
         <v>407</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19317,7 +19373,7 @@
         <v>406</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19325,10 +19381,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19339,7 +19395,7 @@
         <v>151</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19347,10 +19403,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19358,10 +19414,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19372,7 +19428,7 @@
         <v>406</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19383,7 +19439,7 @@
         <v>407</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19440,10 +19496,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19451,10 +19507,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19462,10 +19518,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19473,10 +19529,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>487</v>
+        <v>491</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19484,10 +19540,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19495,10 +19551,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>491</v>
+        <v>495</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19506,10 +19562,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>492</v>
+        <v>496</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>493</v>
+        <v>497</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19517,10 +19573,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>494</v>
+        <v>498</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>495</v>
+        <v>499</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20092,10 +20148,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>496</v>
+        <v>500</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>497</v>
+        <v>501</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>331</v>
@@ -20106,10 +20162,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>498</v>
+        <v>502</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>499</v>
+        <v>503</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>331</v>
@@ -20194,10 +20250,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>500</v>
+        <v>504</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>144</v>
@@ -20208,10 +20264,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>144</v>
@@ -20302,162 +20358,162 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>503</v>
+        <v>507</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>505</v>
+        <v>509</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>506</v>
+        <v>510</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>507</v>
+        <v>511</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>508</v>
+        <v>512</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>509</v>
+        <v>513</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>511</v>
+        <v>515</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>512</v>
+        <v>516</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>514</v>
+        <v>518</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>515</v>
+        <v>519</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>516</v>
+        <v>520</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="16" t="s">
-        <v>517</v>
+        <v>521</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>518</v>
+        <v>522</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="16"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="16" t="s">
-        <v>514</v>
+        <v>518</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="16"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="16" t="s">
-        <v>511</v>
+        <v>515</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="16"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="16" t="s">
-        <v>520</v>
+        <v>524</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="16"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="16" t="s">
-        <v>508</v>
+        <v>512</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="16"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="16" t="s">
-        <v>521</v>
+        <v>525</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="16"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="16" t="s">
-        <v>522</v>
+        <v>526</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="16"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="16" t="s">
+        <v>527</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>523</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>519</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="16"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="16" t="s">
-        <v>505</v>
+        <v>509</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="16"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="16" t="s">
-        <v>524</v>
+        <v>528</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="16"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="16" t="s">
-        <v>525</v>
+        <v>529</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="C18" s="13"/>
       <c r="H18" s="4"/>
@@ -20465,50 +20521,50 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="16" t="s">
-        <v>526</v>
+        <v>530</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="16"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="16" t="s">
-        <v>527</v>
+        <v>531</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="16"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="16" t="s">
-        <v>528</v>
+        <v>532</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="H21" s="4"/>
       <c r="I21" s="16"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="16" t="s">
-        <v>529</v>
+        <v>533</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="H22" s="4"/>
       <c r="I22" s="16"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="16" t="s">
-        <v>530</v>
+        <v>534</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="16"/>
@@ -20545,118 +20601,118 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>531</v>
+        <v>535</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>532</v>
+        <v>536</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>533</v>
+        <v>537</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>534</v>
+        <v>538</v>
       </c>
       <c r="B2" s="4" t="n">
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>535</v>
+        <v>539</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>534</v>
+        <v>538</v>
       </c>
       <c r="B3" s="4" t="n">
         <v>2</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>536</v>
+        <v>540</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>534</v>
+        <v>538</v>
       </c>
       <c r="B4" s="4" t="n">
         <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>537</v>
+        <v>541</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>534</v>
+        <v>538</v>
       </c>
       <c r="B5" s="4" t="n">
         <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>538</v>
+        <v>542</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>534</v>
+        <v>538</v>
       </c>
       <c r="B6" s="4" t="n">
         <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>539</v>
+        <v>543</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>534</v>
+        <v>538</v>
       </c>
       <c r="B7" s="4" t="n">
         <v>6</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="16"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>534</v>
+        <v>538</v>
       </c>
       <c r="B8" s="4" t="n">
         <v>7</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="16"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>534</v>
+        <v>538</v>
       </c>
       <c r="B9" s="4" t="n">
         <v>8</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="16"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>541</v>
+        <v>545</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>70</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>542</v>
+        <v>546</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="16"/>
@@ -20668,30 +20724,30 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>543</v>
+        <v>547</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>533</v>
+        <v>537</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="16"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>544</v>
+        <v>548</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>545</v>
+        <v>549</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="16"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>546</v>
+        <v>550</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>547</v>
+        <v>551</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="16"/>
@@ -20893,7 +20949,7 @@
         <v>155</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>497</v>
+        <v>501</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>266</v>
@@ -20907,7 +20963,7 @@
         <v>158</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>499</v>
+        <v>503</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>266</v>
@@ -20935,7 +20991,7 @@
         <v>155</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>497</v>
+        <v>501</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>266</v>
@@ -20949,7 +21005,7 @@
         <v>158</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>499</v>
+        <v>503</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>266</v>
@@ -21134,7 +21190,7 @@
         <v>254</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>548</v>
+        <v>552</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21148,7 +21204,7 @@
         <v>255</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>548</v>
+        <v>552</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21162,7 +21218,7 @@
         <v>256</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>548</v>
+        <v>552</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -21176,7 +21232,7 @@
         <v>156</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>548</v>
+        <v>552</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -21190,7 +21246,7 @@
         <v>252</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>548</v>
+        <v>552</v>
       </c>
     </row>
   </sheetData>
@@ -21243,10 +21299,10 @@
         <v>151</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>549</v>
+        <v>553</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>550</v>
+        <v>554</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21254,13 +21310,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>551</v>
+        <v>555</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>150</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>550</v>
+        <v>554</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21271,10 +21327,10 @@
         <v>231</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>552</v>
+        <v>556</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>550</v>
+        <v>554</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -21285,10 +21341,10 @@
         <v>233</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>553</v>
+        <v>557</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>550</v>
+        <v>554</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -21299,10 +21355,10 @@
         <v>151</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>554</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -21316,7 +21372,7 @@
         <v>148</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>550</v>
+        <v>554</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -21327,10 +21383,10 @@
         <v>142</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>555</v>
+        <v>559</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>550</v>
+        <v>554</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -21344,7 +21400,7 @@
         <v>146</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>550</v>
+        <v>554</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -21355,10 +21411,10 @@
         <v>327</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>556</v>
+        <v>560</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>550</v>
+        <v>554</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -21369,10 +21425,10 @@
         <v>325</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>556</v>
+        <v>560</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>550</v>
+        <v>554</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -21418,7 +21474,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L25" activeCellId="0" sqref="L25"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21444,10 +21500,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>557</v>
+        <v>561</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>558</v>
+        <v>562</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21455,10 +21511,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>559</v>
+        <v>563</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>560</v>
+        <v>564</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21466,10 +21522,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>561</v>
+        <v>565</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>562</v>
+        <v>566</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21477,10 +21533,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>563</v>
+        <v>567</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>564</v>
+        <v>568</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21488,10 +21544,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>566</v>
+        <v>570</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21499,10 +21555,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>567</v>
+        <v>571</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>568</v>
+        <v>572</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21513,7 +21569,7 @@
         <v>160</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>569</v>
+        <v>573</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21524,7 +21580,7 @@
         <v>160</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>569</v>
+        <v>573</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Deployed e7a6e4e2 with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/Manual/source/tab/connectors.xlsx
+++ b/Manual/source/tab/connectors.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="51"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="rozcestnik" sheetId="1" state="visible" r:id="rId3"/>
@@ -975,13 +975,13 @@
     <t xml:space="preserve">+24V DC napájení brzdy</t>
   </si>
   <si>
+    <t xml:space="preserve">+ Brzda servomotoru</t>
+  </si>
+  <si>
     <t xml:space="preserve">VCCD</t>
   </si>
   <si>
     <t xml:space="preserve">+24V DC napájení diag. brzdy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+ Brzda servomotoru</t>
   </si>
   <si>
     <t xml:space="preserve">- Brzda servomotoru</t>
@@ -14235,10 +14235,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14282,10 +14282,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>283</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>284</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>279</v>
@@ -14296,7 +14296,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>258</v>
+        <v>284</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>285</v>
@@ -14318,6 +14318,10 @@
       <c r="D5" s="4" t="s">
         <v>279</v>
       </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0"/>
+      <c r="C9" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -18301,7 +18305,7 @@
   </sheetPr>
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>

</xml_diff>